<commit_message>
Changes of get the Quote time
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="349">
   <si>
     <t>Sno</t>
   </si>
@@ -998,6 +998,69 @@
   </si>
   <si>
     <t>320018253354</t>
+  </si>
+  <si>
+    <t>320018256721</t>
+  </si>
+  <si>
+    <t>320018256732</t>
+  </si>
+  <si>
+    <t>320018256765</t>
+  </si>
+  <si>
+    <t>320018256787</t>
+  </si>
+  <si>
+    <t>320018256824</t>
+  </si>
+  <si>
+    <t>320018256846</t>
+  </si>
+  <si>
+    <t>320018256879</t>
+  </si>
+  <si>
+    <t>320018256890</t>
+  </si>
+  <si>
+    <t>320018256927</t>
+  </si>
+  <si>
+    <t>320018256949</t>
+  </si>
+  <si>
+    <t>320018256982</t>
+  </si>
+  <si>
+    <t>320018257007</t>
+  </si>
+  <si>
+    <t>320018257030</t>
+  </si>
+  <si>
+    <t>320018257051</t>
+  </si>
+  <si>
+    <t>320018257084</t>
+  </si>
+  <si>
+    <t>320018257100</t>
+  </si>
+  <si>
+    <t>320018257143</t>
+  </si>
+  <si>
+    <t>320018257165</t>
+  </si>
+  <si>
+    <t>320018257198</t>
+  </si>
+  <si>
+    <t>320018257213</t>
+  </si>
+  <si>
+    <t>320018257246</t>
   </si>
 </sst>
 </file>
@@ -1390,7 +1453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1454,7 +1517,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>307</v>
+        <v>328</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="2"/>
@@ -1475,7 +1538,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>308</v>
+        <v>329</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="2"/>
@@ -1496,7 +1559,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="2"/>
@@ -1519,10 +1582,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="D5" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1544,10 +1607,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="D6" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1569,10 +1632,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="D7" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1592,7 +1655,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -1613,7 +1676,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>335</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -1634,7 +1697,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>336</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -1655,7 +1718,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>316</v>
+        <v>337</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -1676,7 +1739,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>317</v>
+        <v>338</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -1699,10 +1762,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="D13" t="s">
-        <v>318</v>
+        <v>339</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1722,10 +1785,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="D14" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1745,10 +1808,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="D15" t="s">
-        <v>320</v>
+        <v>341</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1768,10 +1831,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="D16" t="s">
-        <v>321</v>
+        <v>342</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1791,10 +1854,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="D17" t="s">
-        <v>322</v>
+        <v>343</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1814,7 +1877,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>344</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -1837,7 +1900,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2"/>
@@ -1858,7 +1921,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>325</v>
+        <v>346</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="2"/>
@@ -1879,7 +1942,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>326</v>
+        <v>347</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="2"/>
@@ -1902,7 +1965,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>327</v>
+        <v>348</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 6th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="197">
   <si>
     <t>Sno</t>
   </si>
@@ -506,6 +506,105 @@
   </si>
   <si>
     <t>320018472127</t>
+  </si>
+  <si>
+    <t>320018475181</t>
+  </si>
+  <si>
+    <t>320018475207</t>
+  </si>
+  <si>
+    <t>320018475230</t>
+  </si>
+  <si>
+    <t>320018475251</t>
+  </si>
+  <si>
+    <t>320018475295</t>
+  </si>
+  <si>
+    <t>320018475310</t>
+  </si>
+  <si>
+    <t>320018475343</t>
+  </si>
+  <si>
+    <t>320018475365</t>
+  </si>
+  <si>
+    <t>320018475402</t>
+  </si>
+  <si>
+    <t>320018475435</t>
+  </si>
+  <si>
+    <t>320018475479</t>
+  </si>
+  <si>
+    <t>320018475505</t>
+  </si>
+  <si>
+    <t>320018475538</t>
+  </si>
+  <si>
+    <t>320018475550</t>
+  </si>
+  <si>
+    <t>320018475582</t>
+  </si>
+  <si>
+    <t>320018475696</t>
+  </si>
+  <si>
+    <t>320018475733</t>
+  </si>
+  <si>
+    <t>320018475766</t>
+  </si>
+  <si>
+    <t>320018475799</t>
+  </si>
+  <si>
+    <t>320018475836</t>
+  </si>
+  <si>
+    <t>320018475869</t>
+  </si>
+  <si>
+    <t>320018482919</t>
+  </si>
+  <si>
+    <t>320018483205</t>
+  </si>
+  <si>
+    <t>320018483238</t>
+  </si>
+  <si>
+    <t>320018483260</t>
+  </si>
+  <si>
+    <t>320018483282</t>
+  </si>
+  <si>
+    <t>320018483330</t>
+  </si>
+  <si>
+    <t>320018483352</t>
+  </si>
+  <si>
+    <t>320018483385</t>
+  </si>
+  <si>
+    <t>320018483411</t>
+  </si>
+  <si>
+    <t>320018483444</t>
+  </si>
+  <si>
+    <t>320018483466</t>
+  </si>
+  <si>
+    <t>320018483503</t>
   </si>
 </sst>
 </file>
@@ -1082,7 +1181,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>186</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1132,7 +1231,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>187</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1174,7 +1273,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>188</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1226,10 +1325,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1280,10 +1379,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -1338,10 +1437,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -1400,7 +1499,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>192</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -1456,7 +1555,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -1496,7 +1595,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -1536,7 +1635,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -1576,7 +1675,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -1618,10 +1717,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1660,10 +1759,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -1702,10 +1801,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -1744,10 +1843,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -1786,10 +1885,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -1828,7 +1927,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -1870,7 +1969,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -1910,7 +2009,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -1950,7 +2049,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -1992,7 +2091,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
changes of 23rd may 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2559" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="427">
   <si>
     <t>Sno</t>
   </si>
@@ -1232,6 +1232,69 @@
   </si>
   <si>
     <t>320018586619</t>
+  </si>
+  <si>
+    <t>320018606316</t>
+  </si>
+  <si>
+    <t>320018606327</t>
+  </si>
+  <si>
+    <t>320018606350</t>
+  </si>
+  <si>
+    <t>320018606371</t>
+  </si>
+  <si>
+    <t>320018606419</t>
+  </si>
+  <si>
+    <t>320018606430</t>
+  </si>
+  <si>
+    <t>320018606463</t>
+  </si>
+  <si>
+    <t>320018606485</t>
+  </si>
+  <si>
+    <t>320018606511</t>
+  </si>
+  <si>
+    <t>320018606533</t>
+  </si>
+  <si>
+    <t>320018606577</t>
+  </si>
+  <si>
+    <t>320018606599</t>
+  </si>
+  <si>
+    <t>320018606625</t>
+  </si>
+  <si>
+    <t>320018606647</t>
+  </si>
+  <si>
+    <t>320018606670</t>
+  </si>
+  <si>
+    <t>320018606691</t>
+  </si>
+  <si>
+    <t>320018606739</t>
+  </si>
+  <si>
+    <t>320018606750</t>
+  </si>
+  <si>
+    <t>320018606783</t>
+  </si>
+  <si>
+    <t>320018606809</t>
+  </si>
+  <si>
+    <t>320018606831</t>
   </si>
 </sst>
 </file>
@@ -1674,7 +1737,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD24"/>
+  <dimension ref="A1:AE24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1808,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>385</v>
+        <v>406</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1858,7 +1921,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>386</v>
+        <v>407</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1900,7 +1963,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>387</v>
+        <v>408</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -1952,10 +2015,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>388</v>
+        <v>409</v>
       </c>
       <c r="D5" t="s">
-        <v>388</v>
+        <v>409</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2006,10 +2069,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="D6" t="s">
-        <v>389</v>
+        <v>410</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2064,10 +2127,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
       <c r="D7" t="s">
-        <v>390</v>
+        <v>411</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2128,7 +2191,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>391</v>
+        <v>412</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2184,7 +2247,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>392</v>
+        <v>413</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2224,7 +2287,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>393</v>
+        <v>414</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2264,7 +2327,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>394</v>
+        <v>415</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2304,7 +2367,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2346,10 +2409,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>417</v>
       </c>
       <c r="D13" t="s">
-        <v>396</v>
+        <v>417</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2400,10 +2463,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>397</v>
+        <v>418</v>
       </c>
       <c r="D14" t="s">
-        <v>397</v>
+        <v>418</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2454,10 +2517,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="D15" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2508,10 +2571,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="D16" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2562,10 +2625,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="D17" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2616,7 +2679,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>401</v>
+        <v>422</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2658,7 +2721,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>402</v>
+        <v>423</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2710,7 +2773,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>403</v>
+        <v>424</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2762,7 +2825,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>404</v>
+        <v>425</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2816,7 +2879,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>405</v>
+        <v>426</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 24th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2664" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="450">
   <si>
     <t>Sno</t>
   </si>
@@ -1295,6 +1295,75 @@
   </si>
   <si>
     <t>320018606831</t>
+  </si>
+  <si>
+    <t>320018621062</t>
+  </si>
+  <si>
+    <t>320018621073</t>
+  </si>
+  <si>
+    <t>320018621100</t>
+  </si>
+  <si>
+    <t>320018621121</t>
+  </si>
+  <si>
+    <t>320018621165</t>
+  </si>
+  <si>
+    <t>320018621187</t>
+  </si>
+  <si>
+    <t>320018621213</t>
+  </si>
+  <si>
+    <t>320018621235</t>
+  </si>
+  <si>
+    <t>320018621268</t>
+  </si>
+  <si>
+    <t>320018621280</t>
+  </si>
+  <si>
+    <t>320018621327</t>
+  </si>
+  <si>
+    <t>320018621349</t>
+  </si>
+  <si>
+    <t>320018621371</t>
+  </si>
+  <si>
+    <t>320018621393</t>
+  </si>
+  <si>
+    <t>320018621420</t>
+  </si>
+  <si>
+    <t>320018621441</t>
+  </si>
+  <si>
+    <t>320018621485</t>
+  </si>
+  <si>
+    <t>320018621500</t>
+  </si>
+  <si>
+    <t>320018621533</t>
+  </si>
+  <si>
+    <t>320018621555</t>
+  </si>
+  <si>
+    <t>320018621588</t>
+  </si>
+  <si>
+    <t>320018624006</t>
+  </si>
+  <si>
+    <t>320018624657</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>406</v>
+        <v>449</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1921,7 +1990,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>407</v>
+        <v>428</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -1963,7 +2032,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>408</v>
+        <v>429</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -2015,10 +2084,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>409</v>
+        <v>430</v>
       </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>430</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2069,10 +2138,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>410</v>
+        <v>431</v>
       </c>
       <c r="D6" t="s">
-        <v>410</v>
+        <v>431</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2127,10 +2196,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>411</v>
+        <v>432</v>
       </c>
       <c r="D7" t="s">
-        <v>411</v>
+        <v>432</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2191,7 +2260,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>412</v>
+        <v>433</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2247,7 +2316,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>413</v>
+        <v>434</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2287,7 +2356,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>414</v>
+        <v>435</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2327,7 +2396,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>415</v>
+        <v>436</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2367,7 +2436,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>416</v>
+        <v>437</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2409,10 +2478,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>417</v>
+        <v>438</v>
       </c>
       <c r="D13" t="s">
-        <v>417</v>
+        <v>438</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2463,10 +2532,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>418</v>
+        <v>439</v>
       </c>
       <c r="D14" t="s">
-        <v>418</v>
+        <v>439</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2517,10 +2586,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
       <c r="D15" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2571,10 +2640,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>420</v>
+        <v>441</v>
       </c>
       <c r="D16" t="s">
-        <v>420</v>
+        <v>441</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2625,10 +2694,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>421</v>
+        <v>442</v>
       </c>
       <c r="D17" t="s">
-        <v>421</v>
+        <v>442</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2679,7 +2748,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2721,7 +2790,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>423</v>
+        <v>444</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2773,7 +2842,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>424</v>
+        <v>445</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2825,7 +2894,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>425</v>
+        <v>446</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2879,7 +2948,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>426</v>
+        <v>447</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 25th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2786" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="484">
   <si>
     <t>Sno</t>
   </si>
@@ -1364,6 +1364,108 @@
   </si>
   <si>
     <t>320018624657</t>
+  </si>
+  <si>
+    <t>320018624922</t>
+  </si>
+  <si>
+    <t>320018624933</t>
+  </si>
+  <si>
+    <t>320018624966</t>
+  </si>
+  <si>
+    <t>320018624988</t>
+  </si>
+  <si>
+    <t>320018625024</t>
+  </si>
+  <si>
+    <t>320018625046</t>
+  </si>
+  <si>
+    <t>320018625079</t>
+  </si>
+  <si>
+    <t>320018625090</t>
+  </si>
+  <si>
+    <t>320018625127</t>
+  </si>
+  <si>
+    <t>320018625149</t>
+  </si>
+  <si>
+    <t>320018625182</t>
+  </si>
+  <si>
+    <t>320018625220</t>
+  </si>
+  <si>
+    <t>320018625252</t>
+  </si>
+  <si>
+    <t>320018625274</t>
+  </si>
+  <si>
+    <t>320018625300</t>
+  </si>
+  <si>
+    <t>320018625322</t>
+  </si>
+  <si>
+    <t>320018625366</t>
+  </si>
+  <si>
+    <t>320018625388</t>
+  </si>
+  <si>
+    <t>320018625414</t>
+  </si>
+  <si>
+    <t>320018625436</t>
+  </si>
+  <si>
+    <t>320018625469</t>
+  </si>
+  <si>
+    <t>320018628560</t>
+  </si>
+  <si>
+    <t>320018628571</t>
+  </si>
+  <si>
+    <t>320018628608</t>
+  </si>
+  <si>
+    <t>320018628620</t>
+  </si>
+  <si>
+    <t>320018628663</t>
+  </si>
+  <si>
+    <t>320018628685</t>
+  </si>
+  <si>
+    <t>320018628711</t>
+  </si>
+  <si>
+    <t>320018628733</t>
+  </si>
+  <si>
+    <t>320018628766</t>
+  </si>
+  <si>
+    <t>320018628788</t>
+  </si>
+  <si>
+    <t>320018628825</t>
+  </si>
+  <si>
+    <t>320018628847</t>
+  </si>
+  <si>
+    <t>320018628870</t>
   </si>
 </sst>
 </file>
@@ -1806,7 +1908,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE24"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
@@ -1940,7 +2042,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>449</v>
+        <v>471</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -1990,7 +2092,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>428</v>
+        <v>472</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -2032,7 +2134,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>473</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -2084,10 +2186,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>430</v>
+        <v>474</v>
       </c>
       <c r="D5" t="s">
-        <v>430</v>
+        <v>474</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2138,10 +2240,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>431</v>
+        <v>475</v>
       </c>
       <c r="D6" t="s">
-        <v>431</v>
+        <v>475</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2196,10 +2298,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>432</v>
+        <v>476</v>
       </c>
       <c r="D7" t="s">
-        <v>432</v>
+        <v>476</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2260,7 +2362,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>433</v>
+        <v>477</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2316,7 +2418,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>434</v>
+        <v>478</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2356,7 +2458,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>435</v>
+        <v>479</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2396,7 +2498,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>436</v>
+        <v>480</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2436,7 +2538,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>437</v>
+        <v>481</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2478,10 +2580,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>438</v>
+        <v>482</v>
       </c>
       <c r="D13" t="s">
-        <v>438</v>
+        <v>482</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2532,10 +2634,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>439</v>
+        <v>483</v>
       </c>
       <c r="D14" t="s">
-        <v>439</v>
+        <v>483</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2586,10 +2688,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="D15" t="s">
-        <v>440</v>
+        <v>463</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2640,10 +2742,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="D16" t="s">
-        <v>441</v>
+        <v>464</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2694,10 +2796,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>442</v>
+        <v>465</v>
       </c>
       <c r="D17" t="s">
-        <v>442</v>
+        <v>465</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2748,7 +2850,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>443</v>
+        <v>466</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2790,7 +2892,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>444</v>
+        <v>467</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2842,7 +2944,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>445</v>
+        <v>468</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2894,7 +2996,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>446</v>
+        <v>469</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -2948,7 +3050,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>447</v>
+        <v>470</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>

<commit_message>
Changes of 26th May 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
+++ b/FedExApplication/src/TestFiles/CheetahProcessing.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3119" uniqueCount="526">
   <si>
     <t>Sno</t>
   </si>
@@ -1466,6 +1466,132 @@
   </si>
   <si>
     <t>320018628870</t>
+  </si>
+  <si>
+    <t>320018630457</t>
+  </si>
+  <si>
+    <t>320018630468</t>
+  </si>
+  <si>
+    <t>320018630490</t>
+  </si>
+  <si>
+    <t>320018630733</t>
+  </si>
+  <si>
+    <t>320018630777</t>
+  </si>
+  <si>
+    <t>320018630799</t>
+  </si>
+  <si>
+    <t>320018630825</t>
+  </si>
+  <si>
+    <t>320018630847</t>
+  </si>
+  <si>
+    <t>320018630870</t>
+  </si>
+  <si>
+    <t>320018630891</t>
+  </si>
+  <si>
+    <t>320018630939</t>
+  </si>
+  <si>
+    <t>320018630950</t>
+  </si>
+  <si>
+    <t>320018630983</t>
+  </si>
+  <si>
+    <t>320018631008</t>
+  </si>
+  <si>
+    <t>320018631030</t>
+  </si>
+  <si>
+    <t>320018631063</t>
+  </si>
+  <si>
+    <t>320018631100</t>
+  </si>
+  <si>
+    <t>320018631133</t>
+  </si>
+  <si>
+    <t>320018631177</t>
+  </si>
+  <si>
+    <t>320018631199</t>
+  </si>
+  <si>
+    <t>320018631225</t>
+  </si>
+  <si>
+    <t>320018638745</t>
+  </si>
+  <si>
+    <t>320018638756</t>
+  </si>
+  <si>
+    <t>320018638789</t>
+  </si>
+  <si>
+    <t>320018638804</t>
+  </si>
+  <si>
+    <t>320018638848</t>
+  </si>
+  <si>
+    <t>320018638860</t>
+  </si>
+  <si>
+    <t>320018638892</t>
+  </si>
+  <si>
+    <t>320018638918</t>
+  </si>
+  <si>
+    <t>320018638940</t>
+  </si>
+  <si>
+    <t>320018638962</t>
+  </si>
+  <si>
+    <t>320018639009</t>
+  </si>
+  <si>
+    <t>320018639020</t>
+  </si>
+  <si>
+    <t>320018639053</t>
+  </si>
+  <si>
+    <t>320018639075</t>
+  </si>
+  <si>
+    <t>320018639101</t>
+  </si>
+  <si>
+    <t>320018639123</t>
+  </si>
+  <si>
+    <t>320018639167</t>
+  </si>
+  <si>
+    <t>320018639189</t>
+  </si>
+  <si>
+    <t>320018639215</t>
+  </si>
+  <si>
+    <t>320018639237</t>
+  </si>
+  <si>
+    <t>320018639260</t>
   </si>
 </sst>
 </file>
@@ -2042,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>471</v>
+        <v>505</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="2"/>
@@ -2092,7 +2218,7 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>506</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="2"/>
@@ -2134,7 +2260,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>473</v>
+        <v>507</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="2"/>
@@ -2186,10 +2312,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>474</v>
+        <v>508</v>
       </c>
       <c r="D5" t="s">
-        <v>474</v>
+        <v>508</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2240,10 +2366,10 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="D6" t="s">
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
@@ -2298,10 +2424,10 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="D7" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
@@ -2362,7 +2488,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
-        <v>477</v>
+        <v>511</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="2"/>
@@ -2418,7 +2544,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
-        <v>478</v>
+        <v>512</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="2"/>
@@ -2458,7 +2584,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
-        <v>479</v>
+        <v>513</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="2"/>
@@ -2498,7 +2624,7 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s">
-        <v>480</v>
+        <v>514</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="2"/>
@@ -2538,7 +2664,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s">
-        <v>481</v>
+        <v>515</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="2"/>
@@ -2580,10 +2706,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>482</v>
+        <v>516</v>
       </c>
       <c r="D13" t="s">
-        <v>482</v>
+        <v>516</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -2634,10 +2760,10 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s">
-        <v>483</v>
+        <v>517</v>
       </c>
       <c r="D14" t="s">
-        <v>483</v>
+        <v>517</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
@@ -2688,10 +2814,10 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s">
-        <v>463</v>
+        <v>518</v>
       </c>
       <c r="D15" t="s">
-        <v>463</v>
+        <v>518</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
@@ -2742,10 +2868,10 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
-        <v>464</v>
+        <v>519</v>
       </c>
       <c r="D16" t="s">
-        <v>464</v>
+        <v>519</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="7" t="s">
@@ -2796,10 +2922,10 @@
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
-        <v>465</v>
+        <v>520</v>
       </c>
       <c r="D17" t="s">
-        <v>465</v>
+        <v>520</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
@@ -2850,7 +2976,7 @@
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="2"/>
@@ -2892,7 +3018,7 @@
         <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>467</v>
+        <v>522</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="2"/>
@@ -2944,7 +3070,7 @@
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s">
-        <v>468</v>
+        <v>523</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="2"/>
@@ -2996,7 +3122,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s">
-        <v>469</v>
+        <v>524</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="2"/>
@@ -3050,7 +3176,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>470</v>
+        <v>525</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="2"/>

</xml_diff>